<commit_message>
Add sample jar and cred files, fix biosamples config handling
</commit_message>
<xml_diff>
--- a/biosamples/BiosampleList.xlsx
+++ b/biosamples/BiosampleList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universidadfv-my.sharepoint.com/personal/7901517_alumnos_ufv_es/Documents/FUB/BO/ENA submission/test/Standard excels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universidadfv-my.sharepoint.com/personal/7901517_alumnos_ufv_es/Documents/FUB/BO/ENA submission/gito/bo-ena/biosamples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="11_F25DC773A252ABDACC104845011C43725ADE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F71562F-D08A-4C8D-B242-580254BEEBA7}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="11_F25DC773A252ABDACC104845011C43725ADE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{23A73473-65A5-4BB9-858A-46829F4FBDC1}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="60">
   <si>
     <t>country</t>
   </si>
@@ -212,6 +212,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -264,7 +267,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -288,6 +291,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -570,54 +576,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.5703125" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
     <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="26.85546875" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" customWidth="1"/>
     <col min="10" max="10" width="30.140625" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" customWidth="1"/>
+    <col min="14" max="14" width="20" customWidth="1"/>
+    <col min="15" max="15" width="28.85546875" customWidth="1"/>
+    <col min="16" max="16" width="19.140625" customWidth="1"/>
+    <col min="17" max="17" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -630,7 +663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B664A9F8-E44F-4C17-BB16-05CEA4160A49}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>

</xml_diff>